<commit_message>
soliutions for Lab 1, ready for Lab 2
</commit_message>
<xml_diff>
--- a/Lemonade.xlsx
+++ b/Lemonade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xronos/now/ms_intro_data_science/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E171B5D6-E677-EC4F-AEE4-52A6FBCD0574}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B4879C-4264-3F49-8092-5302981F5543}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20440" xr2:uid="{E530D8CF-9006-4990-AFF7-605CCCFDACC5}"/>
   </bookViews>
@@ -19,6 +19,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -134,7 +139,40 @@
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -160,19 +198,16 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
@@ -197,17 +232,17 @@
     <sortCondition ref="A1:A366"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A3ABCC81-CAB3-9C4C-B342-07A1AF3E3441}" name="Date" dataDxfId="8" totalsRowDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{9ED8E295-6CE7-024C-83C7-C9FE45A01E6E}" name="Month" dataDxfId="6" totalsRowDxfId="3">
+    <tableColumn id="1" xr3:uid="{A3ABCC81-CAB3-9C4C-B342-07A1AF3E3441}" name="Date" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{9ED8E295-6CE7-024C-83C7-C9FE45A01E6E}" name="Month" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>TEXT(A2, "mmmm")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{BACC8157-5D74-8645-BF13-0901F212CEBF}" name="Day"/>
     <tableColumn id="3" xr3:uid="{BC5F5E37-CAEE-6744-8651-6F3997783B41}" name="Temperature"/>
-    <tableColumn id="4" xr3:uid="{7A7C3784-E071-344E-8F3B-D8B29505ACFB}" name="Rainfall" dataDxfId="7" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{BC855E4F-C0B0-A94B-ACD7-E5DC4BCBF87F}" name="Flyers" totalsRowFunction="sum" totalsRowDxfId="1" totalsRowCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{7A7C3784-E071-344E-8F3B-D8B29505ACFB}" name="Rainfall" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{BC855E4F-C0B0-A94B-ACD7-E5DC4BCBF87F}" name="Flyers" totalsRowFunction="sum" totalsRowDxfId="5" totalsRowCellStyle="Comma"/>
     <tableColumn id="6" xr3:uid="{F9E1C017-AAAF-E642-9339-8332BDC12425}" name="Price"/>
     <tableColumn id="7" xr3:uid="{0C38C40F-D202-7547-ADBA-659FDE162A0D}" name="Sales"/>
-    <tableColumn id="9" xr3:uid="{7C042FD6-2486-CA41-95AF-8B4733F2900C}" name="Revenue" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="0">
+    <tableColumn id="9" xr3:uid="{7C042FD6-2486-CA41-95AF-8B4733F2900C}" name="Revenue" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3">
       <calculatedColumnFormula>G2*H2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -514,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222DEC5F-85B8-47EB-B908-7ED0D2EE7246}">
   <dimension ref="A1:K367"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -524,8 +559,9 @@
     <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10484,7 +10520,7 @@
         <v>43056</v>
       </c>
       <c r="B322" s="1" t="str">
-        <f t="shared" ref="B322:B385" si="10">TEXT(A322, "mmmm")</f>
+        <f t="shared" ref="B322:B366" si="10">TEXT(A322, "mmmm")</f>
         <v>November</v>
       </c>
       <c r="C322" t="s">
@@ -10506,7 +10542,7 @@
         <v>20</v>
       </c>
       <c r="I322" s="4">
-        <f t="shared" ref="I322:I385" si="11">G322*H322</f>
+        <f t="shared" ref="I322:I366" si="11">G322*H322</f>
         <v>6</v>
       </c>
     </row>
@@ -11885,10 +11921,57 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D366">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4948BDC3-18D0-2543-812F-D80B4E4FB873}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4948BDC3-18D0-2543-812F-D80B4E4FB873}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add sales histogram and box/whisker chart
</commit_message>
<xml_diff>
--- a/Lemonade.xlsx
+++ b/Lemonade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xronos/now/ms_intro_data_science/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C72C77-97C1-4045-8BCE-FA5306AA9A2A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A9881E-489D-734C-84B7-C1C4438FF265}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20440" xr2:uid="{E530D8CF-9006-4990-AFF7-605CCCFDACC5}"/>
   </bookViews>
@@ -21,6 +21,20 @@
     <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Lemonade!$H$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Lemonade!$H$2:$H$367</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Lemonade!$H$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Lemonade!$H$2:$H$367</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Lemonade!$H$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Lemonade!$H$2:$H$367</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Lemonade!$H$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Lemonade!$H$2:$H$367</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Lemonade!$H$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Lemonade!$H$2:$H$367</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Lemonade!$H$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Lemonade!$H$2:$H$367</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId8"/>
@@ -8697,6 +8711,141 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Sales</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Sales</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{09B1951D-C609-644A-9067-4A65EB027763}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:v>Sales</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Sales</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Sales</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{B2481735-7BAC-9A4A-AC0A-9B5966DE5DB1}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:v>Sales</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -8897,7 +9046,1110 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9381,1038 +10633,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -10949,6 +11169,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="254">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11466,6 +12718,167 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A2E5C40-1D01-FE4E-8083-E4B839FC8C4B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11874500" y="196850"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02AAD1ED-EC07-B644-A33A-29D855699ED9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16687800" y="196850"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -11503,7 +12916,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11580,7 +12993,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11621,7 +13034,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -16892,8 +18305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222DEC5F-85B8-47EB-B908-7ED0D2EE7246}">
   <dimension ref="A1:L367"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28370,8 +29783,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>

<commit_message>
add rainfall descriptive stats, histogram, and box/whisker chart
</commit_message>
<xml_diff>
--- a/Lemonade.xlsx
+++ b/Lemonade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xronos/now/ms_intro_data_science/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A9881E-489D-734C-84B7-C1C4438FF265}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E8632B-6CF4-354E-A4CC-524434E70854}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20440" xr2:uid="{E530D8CF-9006-4990-AFF7-605CCCFDACC5}"/>
   </bookViews>
@@ -24,16 +24,16 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Lemonade!$H$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Lemonade!$H$2:$H$367</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Lemonade!$H$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Lemonade!$H$2:$H$367</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Lemonade!$H$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Lemonade!$H$2:$H$367</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Lemonade!$E$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Lemonade!$E$2:$E$367</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Lemonade!$E$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Lemonade!$E$2:$E$367</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Lemonade!$H$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Lemonade!$H$2:$H$367</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Lemonade!$H$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Lemonade!$H$2:$H$367</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Lemonade!$H$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Lemonade!$H$2:$H$367</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Lemonade!$E$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Lemonade!$E$2:$E$367</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Lemonade!$E$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Lemonade!$E$2:$E$367</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Std. Dev</t>
+  </si>
+  <si>
+    <t>Rainfall Statistics</t>
   </si>
 </sst>
 </file>
@@ -8783,7 +8786,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8821,8 +8824,143 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B2481735-7BAC-9A4A-AC0A-9B5966DE5DB1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Sales</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Rainfall</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Rainfall</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{E3131B36-99A6-424B-8806-D675D67F52E4}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>Rainfall</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.11</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Rainfall</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Rainfall</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{122B7575-2D88-734D-8280-F31C2EB7A748}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:v>Rainfall</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -9087,6 +9225,86 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10150,6 +10368,1029 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10633,1038 +11874,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -12201,6 +12410,1038 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="254">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12842,6 +14083,162 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="16687800" y="196850"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Chart 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DF9EA5E-E024-434F-AF44-D9D5E851E91B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11849100" y="3244850"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Chart 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97030657-9293-9145-9FFA-4621E858308D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16662400" y="3244850"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -18306,7 +19703,7 @@
   <dimension ref="A1:L367"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18854,7 +20251,7 @@
         <v>5.3999999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>42751</v>
       </c>
@@ -18884,8 +20281,11 @@
         <f t="shared" si="1"/>
         <v>3.5999999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>42752</v>
       </c>
@@ -18915,8 +20315,15 @@
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="2">
+        <f>AVERAGE(E2:E366)</f>
+        <v>0.82660273972602816</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>42753</v>
       </c>
@@ -18946,8 +20353,15 @@
         <f t="shared" si="1"/>
         <v>4.8</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="2">
+        <f>MEDIAN(E2:E366)</f>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>42754</v>
       </c>
@@ -18977,8 +20391,15 @@
         <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20">
+        <f>_xlfn.MODE.SNGL(E2:E366)</f>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>42755</v>
       </c>
@@ -19008,8 +20429,15 @@
         <f t="shared" si="1"/>
         <v>3.5999999999999996</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21">
+        <f>_xlfn.VAR.P(E2:E366)</f>
+        <v>7.4418047663724063E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>42756</v>
       </c>
@@ -19039,8 +20467,15 @@
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22">
+        <f>_xlfn.STDEV.P(E2:E366)</f>
+        <v>0.27279671490640073</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>42757</v>
       </c>
@@ -19071,7 +20506,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>42758</v>
       </c>
@@ -19102,7 +20537,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>42759</v>
       </c>
@@ -19133,7 +20568,7 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>42760</v>
       </c>
@@ -19164,7 +20599,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>42761</v>
       </c>
@@ -19195,7 +20630,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>42762</v>
       </c>
@@ -19226,7 +20661,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>42763</v>
       </c>
@@ -19257,7 +20692,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>42764</v>
       </c>
@@ -19288,7 +20723,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>42765</v>
       </c>
@@ -19319,7 +20754,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>42766</v>
       </c>

</xml_diff>

<commit_message>
add temperature stats, histogram, and box/whisker
</commit_message>
<xml_diff>
--- a/Lemonade.xlsx
+++ b/Lemonade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xronos/now/ms_intro_data_science/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E8632B-6CF4-354E-A4CC-524434E70854}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF63122C-A94C-1D4E-8DAC-DF638D878555}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20440" xr2:uid="{E530D8CF-9006-4990-AFF7-605CCCFDACC5}"/>
   </bookViews>
@@ -26,14 +26,18 @@
     <definedName name="_xlchart.v1.1" hidden="1">Lemonade!$H$2:$H$367</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">Lemonade!$E$1</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Lemonade!$E$2:$E$367</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Lemonade!$E$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Lemonade!$E$2:$E$367</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Lemonade!$H$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Lemonade!$H$2:$H$367</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Lemonade!$E$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Lemonade!$E$2:$E$367</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Lemonade!$E$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Lemonade!$E$2:$E$367</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Lemonade!$D$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Lemonade!$D$2:$D$367</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Lemonade!$D$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Lemonade!$D$2:$D$367</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Lemonade!$D$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Lemonade!$D$2:$D$367</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Lemonade!$E$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Lemonade!$E$2:$E$367</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Lemonade!$H$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Lemonade!$H$2:$H$367</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Lemonade!$D$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Lemonade!$D$2:$D$367</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -53,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -143,6 +147,9 @@
   </si>
   <si>
     <t>Rainfall Statistics</t>
+  </si>
+  <si>
+    <t>Temperature Statistics</t>
   </si>
 </sst>
 </file>
@@ -8786,7 +8793,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8824,7 +8831,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B2481735-7BAC-9A4A-AC0A-9B5966DE5DB1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Sales</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8854,7 +8861,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8892,7 +8899,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{E3131B36-99A6-424B-8806-D675D67F52E4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Rainfall</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8984,7 +8991,222 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Temperature</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Temperature</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{FC989D3A-0B88-E94B-993D-B2AFE84D5E81}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>Temperature</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Temperature</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Temperature</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{0225A343-F5FC-6A4F-8A01-31192C6B1346}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:v>Temperature</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9847,6 +10069,1036 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="254">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr/>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -11391,6 +12643,1029 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11874,1038 +14149,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -13442,18 +14685,18 @@
 </file>
 
 <file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="254">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -13461,16 +14704,16 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -13483,7 +14726,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -13499,7 +14742,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -13507,8 +14750,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -13542,51 +14785,36 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="2">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr/>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="15875" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -13598,30 +14826,27 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
@@ -13641,18 +14866,20 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -13662,7 +14889,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -13671,13 +14898,14 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -13686,17 +14914,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -13705,16 +14933,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -13723,15 +14952,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -13750,16 +14985,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -13768,17 +15004,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -13787,16 +15023,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -13806,8 +15043,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -13817,7 +15054,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -13825,7 +15062,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -13834,21 +15071,10 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -13856,17 +15082,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -13876,26 +15102,27 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -13905,8 +15132,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -13916,19 +15143,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -13938,10 +15166,21 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -13949,8 +15188,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -14239,6 +15484,162 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="16662400" y="3244850"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="7" name="Chart 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A3A4C2D-DE83-EE4A-B8D4-F57E865D5DFD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11861800" y="6470650"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="Chart 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35A901A2-4FF3-B841-9610-FD3CCBB9FA89}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16637000" y="6534150"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -19702,8 +21103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222DEC5F-85B8-47EB-B908-7ED0D2EE7246}">
   <dimension ref="A1:L367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH22" sqref="AH22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20785,7 +22186,7 @@
         <v>5.3999999999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>42767</v>
       </c>
@@ -20816,7 +22217,7 @@
         <v>5.3999999999999995</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>42768</v>
       </c>
@@ -20846,8 +22247,11 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K34" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>42769</v>
       </c>
@@ -20877,8 +22281,15 @@
         <f t="shared" si="1"/>
         <v>6.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K35" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35">
+        <f>AVERAGE(D2:D366)</f>
+        <v>60.731232876712376</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>42770</v>
       </c>
@@ -20908,8 +22319,15 @@
         <f t="shared" si="1"/>
         <v>6.6</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K36" t="s">
+        <v>24</v>
+      </c>
+      <c r="L36">
+        <f>MEDIAN(D2:D366)</f>
+        <v>61.099999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>42771</v>
       </c>
@@ -20939,8 +22357,15 @@
         <f t="shared" si="1"/>
         <v>5.3999999999999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K37" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37">
+        <f>_xlfn.MODE.SNGL(D2:D366)</f>
+        <v>55.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>42772</v>
       </c>
@@ -20970,8 +22395,15 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K38" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38">
+        <f>_xlfn.VAR.P(D2:D366)</f>
+        <v>261.60033957590281</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>42773</v>
       </c>
@@ -21001,8 +22433,15 @@
         <f t="shared" si="1"/>
         <v>6.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K39" t="s">
+        <v>28</v>
+      </c>
+      <c r="L39">
+        <f>_xlfn.STDEV.P(D2:D366)</f>
+        <v>16.174063792872303</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>42774</v>
       </c>
@@ -21033,7 +22472,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>42775</v>
       </c>
@@ -21064,7 +22503,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>42776</v>
       </c>
@@ -21095,7 +22534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42777</v>
       </c>
@@ -21126,7 +22565,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42778</v>
       </c>
@@ -21157,7 +22596,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>42779</v>
       </c>
@@ -21188,7 +22627,7 @@
         <v>5.3999999999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>42780</v>
       </c>
@@ -21219,7 +22658,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>42781</v>
       </c>
@@ -21250,7 +22689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>42782</v>
       </c>

</xml_diff>